<commit_message>
Update student, lecturer, achievement, term, groupLecturer, groupStudent controllers
</commit_message>
<xml_diff>
--- a/public/uploads/evaluations-reviewer.xlsx
+++ b/public/uploads/evaluations-reviewer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450C18DE-663A-4DD3-8709-96F8C86057CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46EC274-9235-49C7-A156-41D529DF2F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>LO</t>
   </si>
   <si>
-    <t>A- Failed</t>
-  </si>
-  <si>
     <t>B-Fair</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t> 20</t>
+  </si>
+  <si>
+    <t>A-Failed</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -696,19 +696,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -716,22 +716,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -739,19 +739,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="G4" s="12">
         <v>10</v>
@@ -762,22 +762,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.3">
@@ -785,22 +785,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="G6" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
@@ -808,22 +808,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" ht="192" customHeight="1" x14ac:dyDescent="0.3">
@@ -831,22 +831,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="G8" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -854,22 +854,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="G9" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.3">
@@ -877,22 +877,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>